<commit_message>
edited formatting and created name column
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acevedoe\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baker/Code/progress_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B532AD56-3015-477F-9A3A-071340D426B4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93339681-71CD-9E41-8607-886C31365F88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="11438" tabRatio="691" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="691" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance Rate" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="26">
   <si>
     <t>Student ID</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Core Course</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +145,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +164,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -254,6 +271,18 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,108 +597,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.86328125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.86328125" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" customWidth="1"/>
-    <col min="4" max="4" width="23.53125" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" style="22" customWidth="1"/>
-    <col min="8" max="8" width="22.1328125" style="23" customWidth="1"/>
-    <col min="9" max="9" width="22.1328125" style="26" customWidth="1"/>
-    <col min="10" max="10" width="22.1328125" style="23" customWidth="1"/>
-    <col min="11" max="11" width="17.86328125" style="22" customWidth="1"/>
-    <col min="12" max="12" width="22.19921875" style="30" customWidth="1"/>
-    <col min="13" max="13" width="7.46484375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" style="23" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="22" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" style="30" customWidth="1"/>
+    <col min="14" max="14" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="29"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2"/>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="29"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="29"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="29"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="29"/>
+      <c r="E5" s="2"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -685,17 +718,17 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.53125" customWidth="1"/>
-    <col min="3" max="3" width="17.53125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.53125" customWidth="1"/>
-    <col min="5" max="6" width="17.53125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="17.53125" style="31" customWidth="1"/>
-    <col min="8" max="10" width="17.53125" style="22" customWidth="1"/>
+    <col min="1" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="6" width="17.5" style="22" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="31" customWidth="1"/>
+    <col min="8" max="10" width="17.5" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -727,7 +760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -739,7 +772,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -751,7 +784,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="29"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -772,22 +805,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.19921875" customWidth="1"/>
-    <col min="2" max="3" width="27.19921875" customWidth="1"/>
-    <col min="4" max="4" width="27.19921875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="27.19921875" customWidth="1"/>
-    <col min="6" max="7" width="27.19921875" style="22" customWidth="1"/>
-    <col min="8" max="8" width="27.19921875" style="31" customWidth="1"/>
-    <col min="9" max="11" width="27.19921875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" customWidth="1"/>
+    <col min="6" max="7" width="27.1640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" style="31" customWidth="1"/>
+    <col min="9" max="11" width="27.1640625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -822,7 +855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
@@ -834,7 +867,7 @@
       <c r="J2" s="20"/>
       <c r="K2" s="29"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
@@ -846,12 +879,12 @@
       <c r="J3" s="20"/>
       <c r="K3" s="29"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="J4" s="20"/>
       <c r="K4" s="29"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
@@ -863,7 +896,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="29"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
@@ -875,7 +908,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="29"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="D7" s="3"/>
       <c r="E7" s="5"/>
@@ -896,21 +929,21 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.86328125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.1328125" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="13.53125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="22.19921875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="12.19921875" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="22" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -942,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
@@ -953,7 +986,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="C3" s="3"/>
       <c r="D3" s="5"/>
@@ -964,7 +997,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
     </row>
   </sheetData>
@@ -975,81 +1008,85 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" style="26" customWidth="1"/>
-    <col min="8" max="8" width="22.1328125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="17.46484375" style="22" customWidth="1"/>
-    <col min="10" max="10" width="17.19921875" style="22" customWidth="1"/>
-    <col min="11" max="11" width="7.46484375" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="22" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="29"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="29"/>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1065,21 +1102,21 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="31" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="23.19921875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="17.19921875" style="23" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
@@ -1122,7 +1159,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1148,21 +1185,21 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.53125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="27.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="20.1328125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="22" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" style="30" customWidth="1"/>
     <col min="10" max="10" width="19.6640625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1231,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
@@ -1205,7 +1242,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1230,21 +1267,21 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="31" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="23.19921875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="17.19921875" style="23" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1276,7 +1313,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
@@ -1287,10 +1324,10 @@
       <c r="I2" s="20"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
     </row>
   </sheetData>
@@ -1300,152 +1337,156 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.796875" customWidth="1"/>
-    <col min="2" max="2" width="33.19921875" style="10" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="8" width="20.6640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="31" customWidth="1"/>
-    <col min="10" max="12" width="20.6640625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="9" width="20.6640625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="31" customWidth="1"/>
+    <col min="11" max="13" width="20.6640625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B2" s="5"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="29"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B3" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B4" s="5"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="29"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B5" s="5"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="29"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B6" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="29"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C4" s="5"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="29"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C5" s="5"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="29"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B7" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="29"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="29"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="29"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="29"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="29"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="29"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="29"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C9" s="5"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="29"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C10" s="5"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1461,17 +1502,17 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.1328125" customWidth="1"/>
-    <col min="3" max="3" width="19.1328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.1328125" customWidth="1"/>
-    <col min="5" max="6" width="19.1328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="19.1328125" customWidth="1"/>
-    <col min="8" max="10" width="19.1328125" style="22" customWidth="1"/>
+    <col min="1" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="6" width="19.1640625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="10" width="19.1640625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1503,7 +1544,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -1515,7 +1556,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1540,7 +1581,7 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="4" customWidth="1"/>
@@ -1550,7 +1591,7 @@
     <col min="8" max="10" width="23.33203125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1582,7 +1623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -1594,7 +1635,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="C3" s="3"/>
       <c r="D3" s="5"/>

</xml_diff>

<commit_message>
updated instructions and excel sheet formatting
</commit_message>
<xml_diff>
--- a/import_template.xlsx
+++ b/import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baker/Code/progress_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93339681-71CD-9E41-8607-886C31365F88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2D2849-D4DF-AE47-9538-197607C19000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="691" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="691" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance Rate" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <t>Core Course</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Name (DELETE!)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -282,7 +282,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +599,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -646,7 +645,7 @@
       <c r="H1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="38" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="24" t="s">
@@ -1011,7 +1010,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1049,7 +1048,7 @@
       <c r="F1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="39" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="24" t="s">
@@ -1339,7 +1338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1355,7 +1356,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="16" t="s">
@@ -1379,7 +1380,7 @@
       <c r="H1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="37" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="24" t="s">

</xml_diff>